<commit_message>
Added choose tract weighted by age group
</commit_message>
<xml_diff>
--- a/TacomaDRT/files/PCAgeEmployment/PCAgeTotals.xlsx
+++ b/TacomaDRT/files/PCAgeEmployment/PCAgeTotals.xlsx
@@ -16,31 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
-  <si>
-    <t>T 0 -14</t>
-  </si>
-  <si>
-    <t>T 15 - 19</t>
-  </si>
-  <si>
-    <t>T 20 - 24</t>
-  </si>
-  <si>
-    <t>T  25 - 34</t>
-  </si>
-  <si>
-    <t>T 35 - 44</t>
-  </si>
-  <si>
-    <t>T 45 - 54</t>
-  </si>
-  <si>
-    <t>T 55 - 64</t>
-  </si>
-  <si>
-    <t>T 65+</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="125">
   <si>
     <t>GEO.id</t>
   </si>
@@ -388,6 +364,33 @@
   </si>
   <si>
     <t>ALL TOTAL</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>0-14</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>55-64</t>
+  </si>
+  <si>
+    <t>65+</t>
   </si>
 </sst>
 </file>
@@ -726,64 +729,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>121</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="L1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>5370000053060200</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2">
         <v>17</v>
@@ -815,13 +818,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>5370000053060300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
       </c>
       <c r="D3">
         <v>431</v>
@@ -853,13 +856,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>5370000053060400</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>703</v>
@@ -891,13 +894,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
         <v>5370000053060500</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
       </c>
       <c r="D5">
         <v>675</v>
@@ -929,13 +932,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>5370000053060600</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
       <c r="D6">
         <v>840</v>
@@ -967,13 +970,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
         <v>5370000053060700</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
       </c>
       <c r="D7">
         <v>768</v>
@@ -1005,13 +1008,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
         <v>5370000053060800</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
       <c r="D8">
         <v>839</v>
@@ -1043,13 +1046,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
         <v>5370000053060900</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
       <c r="D9">
         <v>404</v>
@@ -1081,13 +1084,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
         <v>5370000053060900</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
       <c r="D10">
         <v>1014</v>
@@ -1119,13 +1122,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
         <v>5370000053060900</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
       <c r="D11">
         <v>931</v>
@@ -1157,13 +1160,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
         <v>5370000053060900</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
       </c>
       <c r="D12">
         <v>296</v>
@@ -1195,13 +1198,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
         <v>5370000053061000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
       </c>
       <c r="D13">
         <v>505</v>
@@ -1233,13 +1236,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
         <v>5370000053061000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
       </c>
       <c r="D14">
         <v>561</v>
@@ -1271,13 +1274,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
         <v>5370000053061100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
       </c>
       <c r="D15">
         <v>1056</v>
@@ -1309,13 +1312,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
         <v>5370000053061200</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
       </c>
       <c r="D16">
         <v>856</v>
@@ -1347,13 +1350,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
         <v>5370000053061300</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
       </c>
       <c r="D17">
         <v>1146</v>
@@ -1385,13 +1388,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
         <v>5370000053061400</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
       </c>
       <c r="D18">
         <v>599</v>
@@ -1423,13 +1426,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
         <v>5370000053061500</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
       </c>
       <c r="D19">
         <v>317</v>
@@ -1461,13 +1464,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
         <v>5370000053061600</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
       </c>
       <c r="D20">
         <v>131</v>
@@ -1499,13 +1502,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
         <v>5370000053061600</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
       </c>
       <c r="D21">
         <v>61</v>
@@ -1537,13 +1540,13 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22">
         <v>5370000053061700</v>
-      </c>
-      <c r="C22" t="s">
-        <v>52</v>
       </c>
       <c r="D22">
         <v>972</v>
@@ -1575,13 +1578,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
         <v>5370000053061800</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
       </c>
       <c r="D23">
         <v>635</v>
@@ -1613,13 +1616,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
         <v>5370000053061900</v>
-      </c>
-      <c r="C24" t="s">
-        <v>56</v>
       </c>
       <c r="D24">
         <v>340</v>
@@ -1651,13 +1654,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25">
         <v>5370000053062000</v>
-      </c>
-      <c r="C25" t="s">
-        <v>58</v>
       </c>
       <c r="D25">
         <v>894</v>
@@ -1689,13 +1692,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26">
         <v>5370000053062300</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
       </c>
       <c r="D26">
         <v>1295</v>
@@ -1727,13 +1730,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
         <v>5370000053062400</v>
-      </c>
-      <c r="C27" t="s">
-        <v>62</v>
       </c>
       <c r="D27">
         <v>1134</v>
@@ -1765,13 +1768,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28">
         <v>5370000053062500</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
       </c>
       <c r="D28">
         <v>1456</v>
@@ -1803,13 +1806,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29">
         <v>5370000053062600</v>
-      </c>
-      <c r="C29" t="s">
-        <v>66</v>
       </c>
       <c r="D29">
         <v>669</v>
@@ -1841,13 +1844,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30">
         <v>5370000053062800</v>
-      </c>
-      <c r="C30" t="s">
-        <v>68</v>
       </c>
       <c r="D30">
         <v>1405</v>
@@ -1879,13 +1882,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31">
         <v>5370000053062800</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
       </c>
       <c r="D31">
         <v>926</v>
@@ -1917,13 +1920,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32">
         <v>5370000053062900</v>
-      </c>
-      <c r="C32" t="s">
-        <v>72</v>
       </c>
       <c r="D32">
         <v>1577</v>
@@ -1955,13 +1958,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33">
         <v>5370000053063000</v>
-      </c>
-      <c r="C33" t="s">
-        <v>74</v>
       </c>
       <c r="D33">
         <v>648</v>
@@ -1993,13 +1996,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34">
+        <v>68</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34">
         <v>5370000053063100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
       </c>
       <c r="D34">
         <v>802</v>
@@ -2031,13 +2034,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35">
         <v>5370000053063200</v>
-      </c>
-      <c r="C35" t="s">
-        <v>78</v>
       </c>
       <c r="D35">
         <v>950</v>
@@ -2069,13 +2072,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36">
         <v>5370000053063300</v>
-      </c>
-      <c r="C36" t="s">
-        <v>80</v>
       </c>
       <c r="D36">
         <v>1994</v>
@@ -2107,13 +2110,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37">
         <v>5370000053063400</v>
-      </c>
-      <c r="C37" t="s">
-        <v>82</v>
       </c>
       <c r="D37">
         <v>1623</v>
@@ -2145,13 +2148,13 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38">
         <v>5370000053063500</v>
-      </c>
-      <c r="C38" t="s">
-        <v>84</v>
       </c>
       <c r="D38">
         <v>824</v>
@@ -2183,13 +2186,13 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
         <v>5370000053063500</v>
-      </c>
-      <c r="C39" t="s">
-        <v>86</v>
       </c>
       <c r="D39">
         <v>1211</v>
@@ -2221,13 +2224,13 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40">
         <v>5370000053071600</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
       </c>
       <c r="D40">
         <v>21</v>
@@ -2259,13 +2262,13 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41">
         <v>5370000053071700</v>
-      </c>
-      <c r="C41" t="s">
-        <v>90</v>
       </c>
       <c r="D41">
         <v>520</v>
@@ -2297,13 +2300,13 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42">
         <v>5370000053071700</v>
-      </c>
-      <c r="C42" t="s">
-        <v>92</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -2335,13 +2338,13 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43">
         <v>5370000053071700</v>
-      </c>
-      <c r="C43" t="s">
-        <v>94</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -2373,13 +2376,13 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44">
         <v>5370000053071800</v>
-      </c>
-      <c r="C44" t="s">
-        <v>96</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -2411,13 +2414,13 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45">
         <v>5370000053072300</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -2449,13 +2452,13 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46">
         <v>5370000053072300</v>
-      </c>
-      <c r="C46" t="s">
-        <v>100</v>
       </c>
       <c r="D46">
         <v>350</v>
@@ -2487,13 +2490,13 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47">
         <v>5370000053072310</v>
-      </c>
-      <c r="C47" t="s">
-        <v>102</v>
       </c>
       <c r="D47">
         <v>7</v>
@@ -2525,13 +2528,13 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
-      </c>
-      <c r="B48">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48">
         <v>5370000053072310</v>
-      </c>
-      <c r="C48" t="s">
-        <v>104</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2563,13 +2566,13 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49">
         <v>5370000053072310</v>
-      </c>
-      <c r="C49" t="s">
-        <v>106</v>
       </c>
       <c r="D49">
         <v>329</v>
@@ -2601,13 +2604,13 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50">
         <v>5370000053940000</v>
-      </c>
-      <c r="C50" t="s">
-        <v>108</v>
       </c>
       <c r="D50">
         <v>224</v>
@@ -2639,13 +2642,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>109</v>
-      </c>
-      <c r="B51">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51">
         <v>5370000053940000</v>
-      </c>
-      <c r="C51" t="s">
-        <v>110</v>
       </c>
       <c r="D51">
         <v>38</v>
@@ -2677,13 +2680,13 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>111</v>
-      </c>
-      <c r="B52">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52">
         <v>5370000053940000</v>
-      </c>
-      <c r="C52" t="s">
-        <v>112</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2715,13 +2718,13 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53">
         <v>5370000053940000</v>
-      </c>
-      <c r="C53" t="s">
-        <v>114</v>
       </c>
       <c r="D53">
         <v>1341</v>
@@ -2753,13 +2756,13 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>115</v>
-      </c>
-      <c r="B54">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54">
         <v>5370000053940000</v>
-      </c>
-      <c r="C54" t="s">
-        <v>116</v>
       </c>
       <c r="D54">
         <v>996</v>
@@ -2791,13 +2794,13 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>117</v>
-      </c>
-      <c r="B55">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55">
         <v>5370000053940000</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
       </c>
       <c r="D55">
         <v>819</v>
@@ -2829,13 +2832,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>119</v>
-      </c>
-      <c r="B56">
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56">
         <v>5370000053940000</v>
-      </c>
-      <c r="C56" t="s">
-        <v>120</v>
       </c>
       <c r="D56">
         <v>1238</v>
@@ -2867,13 +2870,13 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
-      </c>
-      <c r="B57">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57">
         <v>5370000053940010</v>
-      </c>
-      <c r="C57" t="s">
-        <v>122</v>
       </c>
       <c r="D57">
         <v>703</v>
@@ -2901,6 +2904,53 @@
       </c>
       <c r="L57">
         <v>4092</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ref="D58:L58" si="0">SUM(D2:D57)</f>
+        <v>38100</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="0"/>
+        <v>13281</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>15732</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>31946</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>26773</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>28182</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>22014</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="0"/>
+        <v>22369</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>198397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>